<commit_message>
Update Import Feature And Add Order Column
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/data/data_import_example.xlsx
+++ b/src/main/resources/assets/data/data_import_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Data Import Template</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,6 +149,10 @@
   </si>
   <si>
     <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -192,18 +196,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,18 +491,19 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.4140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.58203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.58203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.58203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="35.58203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.58203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.58203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.58203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.58203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.58203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.58203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -512,6 +516,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -521,52 +526,58 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -585,11 +596,14 @@
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -598,32 +612,36 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -642,11 +660,14 @@
       <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -655,49 +676,55 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add List Sort Feature And Corresponding Page
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/data/data_import_example.xlsx
+++ b/src/main/resources/assets/data/data_import_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Data Import Template</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,6 +153,26 @@
   </si>
   <si>
     <t>Order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -196,9 +216,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -491,7 +514,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -507,26 +530,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -576,47 +599,47 @@
       <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="2">
-        <v>3</v>
+      <c r="H4" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="3">
-        <v>4</v>
+      <c r="H5" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -640,47 +663,47 @@
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
+      <c r="H7" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="3">
-        <v>5</v>
+      <c r="H8" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -704,19 +727,12 @@
       <c r="G10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="2">
-        <v>2</v>
+      <c r="H10" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="G8:G9"/>
@@ -725,6 +741,13 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>